<commit_message>
Created 1.testGetUser test case in UserTestDDT.java with priority 2 2.ExtentReportListenerClass.java - for Extent Reports 3.testng.xml - to execute test cases
Renamed Reports folder to ExtentReport folder to generate newly executed
test report.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Project\Vinayak_WorkSpace\RestAssuredAutomationFramework\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>UserID</t>
   </si>
@@ -102,13 +98,31 @@
   </si>
   <si>
     <t>Bhalerao</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>Swapnil</t>
+  </si>
+  <si>
+    <t>Gavade</t>
+  </si>
+  <si>
+    <t>d@gmail.com</t>
+  </si>
+  <si>
+    <t>test@4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +141,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,10 +192,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -186,8 +209,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -609,7 +634,34 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>